<commit_message>
updated code as of 31032020
</commit_message>
<xml_diff>
--- a/data/DocProTestData.xlsx
+++ b/data/DocProTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bhuvana\backup 20012020\Updated code\EwQIMS_POM\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OSSGit\CommonFolder\EwQIMS_POM\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="99">
   <si>
     <t>Username</t>
   </si>
@@ -316,6 +316,12 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>Quality Assurance Process and checklists Document</t>
+  </si>
+  <si>
+    <t>(FA)</t>
   </si>
 </sst>
 </file>
@@ -683,7 +689,7 @@
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B7"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -824,7 +830,7 @@
         <v>20</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>18</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -843,8 +849,8 @@
       <c r="E6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F6" t="s">
-        <v>18</v>
+      <c r="F6" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -874,13 +880,13 @@
   <dimension ref="A1:V13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="B3" sqref="B3:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
     <col min="3" max="3" width="83.140625" customWidth="1"/>
     <col min="6" max="6" width="20.28515625" customWidth="1"/>
     <col min="7" max="7" width="18.5703125" customWidth="1"/>
@@ -888,7 +894,7 @@
     <col min="10" max="10" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17" customWidth="1"/>
     <col min="12" max="12" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="47.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="55.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1225,6 +1231,9 @@
       <c r="M11" s="1" t="s">
         <v>77</v>
       </c>
+      <c r="N11" t="s">
+        <v>97</v>
+      </c>
       <c r="O11" t="s">
         <v>60</v>
       </c>
@@ -1233,6 +1242,12 @@
       </c>
       <c r="T11" t="s">
         <v>79</v>
+      </c>
+      <c r="U11" t="s">
+        <v>81</v>
+      </c>
+      <c r="V11" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
@@ -1298,5 +1313,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>